<commit_message>
Fix lint errors; consolidate debug output; remove dead code.
</commit_message>
<xml_diff>
--- a/test-apps/testbed/frontend/performance/performanceResults.xlsx
+++ b/test-apps/testbed/frontend/performance/performanceResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="23">
   <si>
     <t/>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Min Time</t>
+  </si>
+  <si>
+    <t>d:\js\s\imodeljs-core/test-apps/testbed/frontend/performance/imodels/Wraith_MultiMulti.ibim</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R486"/>
+  <dimension ref="A1:R507"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H25" sqref="H25"/>
@@ -27473,6 +27476,1173 @@
         <v>12</v>
       </c>
     </row>
+    <row r="487" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>0</v>
+      </c>
+      <c r="B487" t="s">
+        <v>22</v>
+      </c>
+      <c r="C487" t="s">
+        <v>19</v>
+      </c>
+      <c r="D487" t="s">
+        <v>20</v>
+      </c>
+      <c r="E487">
+        <v>12366</v>
+      </c>
+      <c r="F487">
+        <v>4</v>
+      </c>
+      <c r="G487">
+        <v>1</v>
+      </c>
+      <c r="H487">
+        <v>1</v>
+      </c>
+      <c r="I487">
+        <v>0</v>
+      </c>
+      <c r="J487">
+        <v>0</v>
+      </c>
+      <c r="K487">
+        <v>0</v>
+      </c>
+      <c r="L487">
+        <v>0</v>
+      </c>
+      <c r="M487">
+        <v>5</v>
+      </c>
+      <c r="N487">
+        <v>0</v>
+      </c>
+      <c r="O487">
+        <v>0</v>
+      </c>
+      <c r="P487">
+        <v>11</v>
+      </c>
+      <c r="Q487">
+        <v>0</v>
+      </c>
+      <c r="R487">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="488" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>0</v>
+      </c>
+      <c r="B488" t="s">
+        <v>22</v>
+      </c>
+      <c r="C488" t="s">
+        <v>19</v>
+      </c>
+      <c r="D488" t="s">
+        <v>20</v>
+      </c>
+      <c r="E488">
+        <v>12366</v>
+      </c>
+      <c r="F488">
+        <v>4</v>
+      </c>
+      <c r="G488">
+        <v>0</v>
+      </c>
+      <c r="H488">
+        <v>2</v>
+      </c>
+      <c r="I488">
+        <v>0</v>
+      </c>
+      <c r="J488">
+        <v>0</v>
+      </c>
+      <c r="K488">
+        <v>0</v>
+      </c>
+      <c r="L488">
+        <v>0</v>
+      </c>
+      <c r="M488">
+        <v>8</v>
+      </c>
+      <c r="N488">
+        <v>0</v>
+      </c>
+      <c r="O488">
+        <v>0</v>
+      </c>
+      <c r="P488">
+        <v>14</v>
+      </c>
+      <c r="Q488">
+        <v>0</v>
+      </c>
+      <c r="R488">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="489" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>0</v>
+      </c>
+      <c r="B489" t="s">
+        <v>22</v>
+      </c>
+      <c r="C489" t="s">
+        <v>19</v>
+      </c>
+      <c r="D489" t="s">
+        <v>20</v>
+      </c>
+      <c r="E489">
+        <v>12366</v>
+      </c>
+      <c r="F489">
+        <v>3</v>
+      </c>
+      <c r="G489">
+        <v>0</v>
+      </c>
+      <c r="H489">
+        <v>1</v>
+      </c>
+      <c r="I489">
+        <v>0</v>
+      </c>
+      <c r="J489">
+        <v>0</v>
+      </c>
+      <c r="K489">
+        <v>0</v>
+      </c>
+      <c r="L489">
+        <v>0</v>
+      </c>
+      <c r="M489">
+        <v>5</v>
+      </c>
+      <c r="N489">
+        <v>0</v>
+      </c>
+      <c r="O489">
+        <v>0</v>
+      </c>
+      <c r="P489">
+        <v>9</v>
+      </c>
+      <c r="Q489">
+        <v>0</v>
+      </c>
+      <c r="R489">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="490" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>0</v>
+      </c>
+      <c r="B490" t="s">
+        <v>22</v>
+      </c>
+      <c r="C490" t="s">
+        <v>19</v>
+      </c>
+      <c r="D490" t="s">
+        <v>20</v>
+      </c>
+      <c r="E490">
+        <v>12366</v>
+      </c>
+      <c r="F490">
+        <v>3</v>
+      </c>
+      <c r="G490">
+        <v>0</v>
+      </c>
+      <c r="H490">
+        <v>2</v>
+      </c>
+      <c r="I490">
+        <v>0</v>
+      </c>
+      <c r="J490">
+        <v>0</v>
+      </c>
+      <c r="K490">
+        <v>0</v>
+      </c>
+      <c r="L490">
+        <v>0</v>
+      </c>
+      <c r="M490">
+        <v>5</v>
+      </c>
+      <c r="N490">
+        <v>0</v>
+      </c>
+      <c r="O490">
+        <v>0</v>
+      </c>
+      <c r="P490">
+        <v>10</v>
+      </c>
+      <c r="Q490">
+        <v>0</v>
+      </c>
+      <c r="R490">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="491" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>0</v>
+      </c>
+      <c r="B491" t="s">
+        <v>22</v>
+      </c>
+      <c r="C491" t="s">
+        <v>19</v>
+      </c>
+      <c r="D491" t="s">
+        <v>20</v>
+      </c>
+      <c r="E491">
+        <v>12366</v>
+      </c>
+      <c r="F491">
+        <v>5</v>
+      </c>
+      <c r="G491">
+        <v>0</v>
+      </c>
+      <c r="H491">
+        <v>1</v>
+      </c>
+      <c r="I491">
+        <v>0</v>
+      </c>
+      <c r="J491">
+        <v>0</v>
+      </c>
+      <c r="K491">
+        <v>0</v>
+      </c>
+      <c r="L491">
+        <v>0</v>
+      </c>
+      <c r="M491">
+        <v>12</v>
+      </c>
+      <c r="N491">
+        <v>0</v>
+      </c>
+      <c r="O491">
+        <v>0</v>
+      </c>
+      <c r="P491">
+        <v>18</v>
+      </c>
+      <c r="Q491">
+        <v>0</v>
+      </c>
+      <c r="R491">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="492" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>0</v>
+      </c>
+      <c r="B492" t="s">
+        <v>22</v>
+      </c>
+      <c r="C492" t="s">
+        <v>19</v>
+      </c>
+      <c r="D492" t="s">
+        <v>20</v>
+      </c>
+      <c r="E492">
+        <v>12366</v>
+      </c>
+      <c r="F492">
+        <v>4</v>
+      </c>
+      <c r="G492">
+        <v>0</v>
+      </c>
+      <c r="H492">
+        <v>1</v>
+      </c>
+      <c r="I492">
+        <v>0</v>
+      </c>
+      <c r="J492">
+        <v>0</v>
+      </c>
+      <c r="K492">
+        <v>0</v>
+      </c>
+      <c r="L492">
+        <v>0</v>
+      </c>
+      <c r="M492">
+        <v>4</v>
+      </c>
+      <c r="N492">
+        <v>0</v>
+      </c>
+      <c r="O492">
+        <v>0</v>
+      </c>
+      <c r="P492">
+        <v>9</v>
+      </c>
+      <c r="Q492">
+        <v>0</v>
+      </c>
+      <c r="R492">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="493" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>0</v>
+      </c>
+      <c r="B493" t="s">
+        <v>22</v>
+      </c>
+      <c r="C493" t="s">
+        <v>19</v>
+      </c>
+      <c r="D493" t="s">
+        <v>20</v>
+      </c>
+      <c r="E493">
+        <v>12366</v>
+      </c>
+      <c r="F493">
+        <v>4</v>
+      </c>
+      <c r="G493">
+        <v>0</v>
+      </c>
+      <c r="H493">
+        <v>0</v>
+      </c>
+      <c r="I493">
+        <v>0</v>
+      </c>
+      <c r="J493">
+        <v>0</v>
+      </c>
+      <c r="K493">
+        <v>0</v>
+      </c>
+      <c r="L493">
+        <v>0</v>
+      </c>
+      <c r="M493">
+        <v>7</v>
+      </c>
+      <c r="N493">
+        <v>0</v>
+      </c>
+      <c r="O493">
+        <v>0</v>
+      </c>
+      <c r="P493">
+        <v>11</v>
+      </c>
+      <c r="Q493">
+        <v>0</v>
+      </c>
+      <c r="R493">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="494" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>0</v>
+      </c>
+      <c r="B494" t="s">
+        <v>22</v>
+      </c>
+      <c r="C494" t="s">
+        <v>19</v>
+      </c>
+      <c r="D494" t="s">
+        <v>20</v>
+      </c>
+      <c r="E494">
+        <v>12366</v>
+      </c>
+      <c r="F494">
+        <v>3</v>
+      </c>
+      <c r="G494">
+        <v>0</v>
+      </c>
+      <c r="H494">
+        <v>0</v>
+      </c>
+      <c r="I494">
+        <v>0</v>
+      </c>
+      <c r="J494">
+        <v>0</v>
+      </c>
+      <c r="K494">
+        <v>0</v>
+      </c>
+      <c r="L494">
+        <v>0</v>
+      </c>
+      <c r="M494">
+        <v>6</v>
+      </c>
+      <c r="N494">
+        <v>0</v>
+      </c>
+      <c r="O494">
+        <v>0</v>
+      </c>
+      <c r="P494">
+        <v>9</v>
+      </c>
+      <c r="Q494">
+        <v>0</v>
+      </c>
+      <c r="R494">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="495" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>0</v>
+      </c>
+      <c r="B495" t="s">
+        <v>22</v>
+      </c>
+      <c r="C495" t="s">
+        <v>19</v>
+      </c>
+      <c r="D495" t="s">
+        <v>20</v>
+      </c>
+      <c r="E495">
+        <v>12366</v>
+      </c>
+      <c r="F495">
+        <v>3</v>
+      </c>
+      <c r="G495">
+        <v>0</v>
+      </c>
+      <c r="H495">
+        <v>0</v>
+      </c>
+      <c r="I495">
+        <v>1</v>
+      </c>
+      <c r="J495">
+        <v>0</v>
+      </c>
+      <c r="K495">
+        <v>0</v>
+      </c>
+      <c r="L495">
+        <v>0</v>
+      </c>
+      <c r="M495">
+        <v>3</v>
+      </c>
+      <c r="N495">
+        <v>0</v>
+      </c>
+      <c r="O495">
+        <v>0</v>
+      </c>
+      <c r="P495">
+        <v>7</v>
+      </c>
+      <c r="Q495">
+        <v>0</v>
+      </c>
+      <c r="R495">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="496" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>0</v>
+      </c>
+      <c r="B496" t="s">
+        <v>22</v>
+      </c>
+      <c r="C496" t="s">
+        <v>19</v>
+      </c>
+      <c r="D496" t="s">
+        <v>20</v>
+      </c>
+      <c r="E496">
+        <v>12366</v>
+      </c>
+      <c r="F496">
+        <v>3</v>
+      </c>
+      <c r="G496">
+        <v>0</v>
+      </c>
+      <c r="H496">
+        <v>0</v>
+      </c>
+      <c r="I496">
+        <v>0</v>
+      </c>
+      <c r="J496">
+        <v>0</v>
+      </c>
+      <c r="K496">
+        <v>0</v>
+      </c>
+      <c r="L496">
+        <v>0</v>
+      </c>
+      <c r="M496">
+        <v>5</v>
+      </c>
+      <c r="N496">
+        <v>0</v>
+      </c>
+      <c r="O496">
+        <v>0</v>
+      </c>
+      <c r="P496">
+        <v>8</v>
+      </c>
+      <c r="Q496">
+        <v>0</v>
+      </c>
+      <c r="R496">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="497" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>0</v>
+      </c>
+      <c r="B497" t="s">
+        <v>22</v>
+      </c>
+      <c r="C497" t="s">
+        <v>19</v>
+      </c>
+      <c r="D497" t="s">
+        <v>20</v>
+      </c>
+      <c r="E497">
+        <v>12366</v>
+      </c>
+      <c r="F497">
+        <v>3</v>
+      </c>
+      <c r="G497">
+        <v>0</v>
+      </c>
+      <c r="H497">
+        <v>1</v>
+      </c>
+      <c r="I497">
+        <v>0</v>
+      </c>
+      <c r="J497">
+        <v>0</v>
+      </c>
+      <c r="K497">
+        <v>0</v>
+      </c>
+      <c r="L497">
+        <v>0</v>
+      </c>
+      <c r="M497">
+        <v>5</v>
+      </c>
+      <c r="N497">
+        <v>0</v>
+      </c>
+      <c r="O497">
+        <v>0</v>
+      </c>
+      <c r="P497">
+        <v>9</v>
+      </c>
+      <c r="Q497">
+        <v>0</v>
+      </c>
+      <c r="R497">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="498" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>0</v>
+      </c>
+      <c r="B498" t="s">
+        <v>22</v>
+      </c>
+      <c r="C498" t="s">
+        <v>19</v>
+      </c>
+      <c r="D498" t="s">
+        <v>20</v>
+      </c>
+      <c r="E498">
+        <v>12366</v>
+      </c>
+      <c r="F498">
+        <v>3</v>
+      </c>
+      <c r="G498">
+        <v>0</v>
+      </c>
+      <c r="H498">
+        <v>1</v>
+      </c>
+      <c r="I498">
+        <v>0</v>
+      </c>
+      <c r="J498">
+        <v>0</v>
+      </c>
+      <c r="K498">
+        <v>0</v>
+      </c>
+      <c r="L498">
+        <v>0</v>
+      </c>
+      <c r="M498">
+        <v>3</v>
+      </c>
+      <c r="N498">
+        <v>0</v>
+      </c>
+      <c r="O498">
+        <v>0</v>
+      </c>
+      <c r="P498">
+        <v>7</v>
+      </c>
+      <c r="Q498">
+        <v>0</v>
+      </c>
+      <c r="R498">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="499" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>0</v>
+      </c>
+      <c r="B499" t="s">
+        <v>22</v>
+      </c>
+      <c r="C499" t="s">
+        <v>19</v>
+      </c>
+      <c r="D499" t="s">
+        <v>20</v>
+      </c>
+      <c r="E499">
+        <v>12366</v>
+      </c>
+      <c r="F499">
+        <v>3</v>
+      </c>
+      <c r="G499">
+        <v>0</v>
+      </c>
+      <c r="H499">
+        <v>0</v>
+      </c>
+      <c r="I499">
+        <v>1</v>
+      </c>
+      <c r="J499">
+        <v>0</v>
+      </c>
+      <c r="K499">
+        <v>0</v>
+      </c>
+      <c r="L499">
+        <v>0</v>
+      </c>
+      <c r="M499">
+        <v>3</v>
+      </c>
+      <c r="N499">
+        <v>0</v>
+      </c>
+      <c r="O499">
+        <v>0</v>
+      </c>
+      <c r="P499">
+        <v>7</v>
+      </c>
+      <c r="Q499">
+        <v>0</v>
+      </c>
+      <c r="R499">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="500" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>0</v>
+      </c>
+      <c r="B500" t="s">
+        <v>22</v>
+      </c>
+      <c r="C500" t="s">
+        <v>19</v>
+      </c>
+      <c r="D500" t="s">
+        <v>20</v>
+      </c>
+      <c r="E500">
+        <v>12366</v>
+      </c>
+      <c r="F500">
+        <v>3</v>
+      </c>
+      <c r="G500">
+        <v>0</v>
+      </c>
+      <c r="H500">
+        <v>1</v>
+      </c>
+      <c r="I500">
+        <v>0</v>
+      </c>
+      <c r="J500">
+        <v>0</v>
+      </c>
+      <c r="K500">
+        <v>0</v>
+      </c>
+      <c r="L500">
+        <v>0</v>
+      </c>
+      <c r="M500">
+        <v>4</v>
+      </c>
+      <c r="N500">
+        <v>0</v>
+      </c>
+      <c r="O500">
+        <v>0</v>
+      </c>
+      <c r="P500">
+        <v>8</v>
+      </c>
+      <c r="Q500">
+        <v>0</v>
+      </c>
+      <c r="R500">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="501" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>0</v>
+      </c>
+      <c r="B501" t="s">
+        <v>22</v>
+      </c>
+      <c r="C501" t="s">
+        <v>19</v>
+      </c>
+      <c r="D501" t="s">
+        <v>20</v>
+      </c>
+      <c r="E501">
+        <v>12366</v>
+      </c>
+      <c r="F501">
+        <v>5</v>
+      </c>
+      <c r="G501">
+        <v>0</v>
+      </c>
+      <c r="H501">
+        <v>0</v>
+      </c>
+      <c r="I501">
+        <v>1</v>
+      </c>
+      <c r="J501">
+        <v>0</v>
+      </c>
+      <c r="K501">
+        <v>0</v>
+      </c>
+      <c r="L501">
+        <v>0</v>
+      </c>
+      <c r="M501">
+        <v>3</v>
+      </c>
+      <c r="N501">
+        <v>0</v>
+      </c>
+      <c r="O501">
+        <v>0</v>
+      </c>
+      <c r="P501">
+        <v>9</v>
+      </c>
+      <c r="Q501">
+        <v>0</v>
+      </c>
+      <c r="R501">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="502" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>0</v>
+      </c>
+      <c r="B502" t="s">
+        <v>22</v>
+      </c>
+      <c r="C502" t="s">
+        <v>19</v>
+      </c>
+      <c r="D502" t="s">
+        <v>20</v>
+      </c>
+      <c r="E502">
+        <v>12366</v>
+      </c>
+      <c r="F502">
+        <v>3</v>
+      </c>
+      <c r="G502">
+        <v>0</v>
+      </c>
+      <c r="H502">
+        <v>0</v>
+      </c>
+      <c r="I502">
+        <v>0</v>
+      </c>
+      <c r="J502">
+        <v>0</v>
+      </c>
+      <c r="K502">
+        <v>0</v>
+      </c>
+      <c r="L502">
+        <v>0</v>
+      </c>
+      <c r="M502">
+        <v>4</v>
+      </c>
+      <c r="N502">
+        <v>0</v>
+      </c>
+      <c r="O502">
+        <v>0</v>
+      </c>
+      <c r="P502">
+        <v>7</v>
+      </c>
+      <c r="Q502">
+        <v>0</v>
+      </c>
+      <c r="R502">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="503" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>0</v>
+      </c>
+      <c r="B503" t="s">
+        <v>22</v>
+      </c>
+      <c r="C503" t="s">
+        <v>19</v>
+      </c>
+      <c r="D503" t="s">
+        <v>20</v>
+      </c>
+      <c r="E503">
+        <v>12366</v>
+      </c>
+      <c r="F503">
+        <v>4</v>
+      </c>
+      <c r="G503">
+        <v>0</v>
+      </c>
+      <c r="H503">
+        <v>0</v>
+      </c>
+      <c r="I503">
+        <v>0</v>
+      </c>
+      <c r="J503">
+        <v>0</v>
+      </c>
+      <c r="K503">
+        <v>0</v>
+      </c>
+      <c r="L503">
+        <v>0</v>
+      </c>
+      <c r="M503">
+        <v>5</v>
+      </c>
+      <c r="N503">
+        <v>0</v>
+      </c>
+      <c r="O503">
+        <v>0</v>
+      </c>
+      <c r="P503">
+        <v>9</v>
+      </c>
+      <c r="Q503">
+        <v>0</v>
+      </c>
+      <c r="R503">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="504" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>0</v>
+      </c>
+      <c r="B504" t="s">
+        <v>22</v>
+      </c>
+      <c r="C504" t="s">
+        <v>19</v>
+      </c>
+      <c r="D504" t="s">
+        <v>20</v>
+      </c>
+      <c r="E504">
+        <v>12366</v>
+      </c>
+      <c r="F504">
+        <v>3</v>
+      </c>
+      <c r="G504">
+        <v>0</v>
+      </c>
+      <c r="H504">
+        <v>0</v>
+      </c>
+      <c r="I504">
+        <v>0</v>
+      </c>
+      <c r="J504">
+        <v>0</v>
+      </c>
+      <c r="K504">
+        <v>0</v>
+      </c>
+      <c r="L504">
+        <v>0</v>
+      </c>
+      <c r="M504">
+        <v>4</v>
+      </c>
+      <c r="N504">
+        <v>0</v>
+      </c>
+      <c r="O504">
+        <v>0</v>
+      </c>
+      <c r="P504">
+        <v>7</v>
+      </c>
+      <c r="Q504">
+        <v>0</v>
+      </c>
+      <c r="R504">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="505" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>0</v>
+      </c>
+      <c r="B505" t="s">
+        <v>22</v>
+      </c>
+      <c r="C505" t="s">
+        <v>19</v>
+      </c>
+      <c r="D505" t="s">
+        <v>20</v>
+      </c>
+      <c r="E505">
+        <v>12366</v>
+      </c>
+      <c r="F505">
+        <v>8</v>
+      </c>
+      <c r="G505">
+        <v>0</v>
+      </c>
+      <c r="H505">
+        <v>1</v>
+      </c>
+      <c r="I505">
+        <v>0</v>
+      </c>
+      <c r="J505">
+        <v>0</v>
+      </c>
+      <c r="K505">
+        <v>0</v>
+      </c>
+      <c r="L505">
+        <v>0</v>
+      </c>
+      <c r="M505">
+        <v>6</v>
+      </c>
+      <c r="N505">
+        <v>0</v>
+      </c>
+      <c r="O505">
+        <v>0</v>
+      </c>
+      <c r="P505">
+        <v>15</v>
+      </c>
+      <c r="Q505">
+        <v>0</v>
+      </c>
+      <c r="R505">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="506" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>0</v>
+      </c>
+      <c r="B506" t="s">
+        <v>22</v>
+      </c>
+      <c r="C506" t="s">
+        <v>19</v>
+      </c>
+      <c r="D506" t="s">
+        <v>20</v>
+      </c>
+      <c r="E506">
+        <v>12366</v>
+      </c>
+      <c r="F506">
+        <v>3</v>
+      </c>
+      <c r="G506">
+        <v>0</v>
+      </c>
+      <c r="H506">
+        <v>0</v>
+      </c>
+      <c r="I506">
+        <v>0</v>
+      </c>
+      <c r="J506">
+        <v>0</v>
+      </c>
+      <c r="K506">
+        <v>0</v>
+      </c>
+      <c r="L506">
+        <v>0</v>
+      </c>
+      <c r="M506">
+        <v>4</v>
+      </c>
+      <c r="N506">
+        <v>0</v>
+      </c>
+      <c r="O506">
+        <v>0</v>
+      </c>
+      <c r="P506">
+        <v>7</v>
+      </c>
+      <c r="Q506">
+        <v>0</v>
+      </c>
+      <c r="R506">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="507" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D507" t="s">
+        <v>21</v>
+      </c>
+      <c r="E507">
+        <v>12366</v>
+      </c>
+      <c r="F507">
+        <v>3</v>
+      </c>
+      <c r="G507">
+        <v>0</v>
+      </c>
+      <c r="H507">
+        <v>0</v>
+      </c>
+      <c r="I507">
+        <v>0</v>
+      </c>
+      <c r="J507">
+        <v>0</v>
+      </c>
+      <c r="K507">
+        <v>0</v>
+      </c>
+      <c r="L507">
+        <v>0</v>
+      </c>
+      <c r="M507">
+        <v>4</v>
+      </c>
+      <c r="N507">
+        <v>0</v>
+      </c>
+      <c r="O507">
+        <v>0</v>
+      </c>
+      <c r="P507">
+        <v>7</v>
+      </c>
+      <c r="Q507">
+        <v>0</v>
+      </c>
+      <c r="R507">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
'Error happened' is not a useful message. We don't need to build a view list - just load the one view we are interested in.
</commit_message>
<xml_diff>
--- a/test-apps/testbed/frontend/performance/performanceResults.xlsx
+++ b/test-apps/testbed/frontend/performance/performanceResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="23">
   <si>
     <t/>
   </si>
@@ -459,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R507"/>
+  <dimension ref="A1:R520"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H25" sqref="H25"/>
@@ -28643,6 +28643,734 @@
         <v>7</v>
       </c>
     </row>
+    <row r="508" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>0</v>
+      </c>
+      <c r="B508" t="s">
+        <v>22</v>
+      </c>
+      <c r="C508" t="s">
+        <v>19</v>
+      </c>
+      <c r="D508" t="s">
+        <v>20</v>
+      </c>
+      <c r="E508">
+        <v>6144</v>
+      </c>
+      <c r="F508">
+        <v>4</v>
+      </c>
+      <c r="G508">
+        <v>0</v>
+      </c>
+      <c r="H508">
+        <v>2</v>
+      </c>
+      <c r="I508">
+        <v>0</v>
+      </c>
+      <c r="J508">
+        <v>0</v>
+      </c>
+      <c r="K508">
+        <v>0</v>
+      </c>
+      <c r="L508">
+        <v>0</v>
+      </c>
+      <c r="M508">
+        <v>13</v>
+      </c>
+      <c r="N508">
+        <v>0</v>
+      </c>
+      <c r="O508">
+        <v>0</v>
+      </c>
+      <c r="P508">
+        <v>19</v>
+      </c>
+      <c r="Q508">
+        <v>0</v>
+      </c>
+      <c r="R508">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="509" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>0</v>
+      </c>
+      <c r="B509" t="s">
+        <v>22</v>
+      </c>
+      <c r="C509" t="s">
+        <v>19</v>
+      </c>
+      <c r="D509" t="s">
+        <v>20</v>
+      </c>
+      <c r="E509">
+        <v>6144</v>
+      </c>
+      <c r="F509">
+        <v>6</v>
+      </c>
+      <c r="G509">
+        <v>0</v>
+      </c>
+      <c r="H509">
+        <v>2</v>
+      </c>
+      <c r="I509">
+        <v>1</v>
+      </c>
+      <c r="J509">
+        <v>0</v>
+      </c>
+      <c r="K509">
+        <v>0</v>
+      </c>
+      <c r="L509">
+        <v>0</v>
+      </c>
+      <c r="M509">
+        <v>15</v>
+      </c>
+      <c r="N509">
+        <v>0</v>
+      </c>
+      <c r="O509">
+        <v>0</v>
+      </c>
+      <c r="P509">
+        <v>24</v>
+      </c>
+      <c r="Q509">
+        <v>0</v>
+      </c>
+      <c r="R509">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="510" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>0</v>
+      </c>
+      <c r="B510" t="s">
+        <v>22</v>
+      </c>
+      <c r="C510" t="s">
+        <v>19</v>
+      </c>
+      <c r="D510" t="s">
+        <v>20</v>
+      </c>
+      <c r="E510">
+        <v>6144</v>
+      </c>
+      <c r="F510">
+        <v>4</v>
+      </c>
+      <c r="G510">
+        <v>0</v>
+      </c>
+      <c r="H510">
+        <v>2</v>
+      </c>
+      <c r="I510">
+        <v>0</v>
+      </c>
+      <c r="J510">
+        <v>0</v>
+      </c>
+      <c r="K510">
+        <v>0</v>
+      </c>
+      <c r="L510">
+        <v>0</v>
+      </c>
+      <c r="M510">
+        <v>14</v>
+      </c>
+      <c r="N510">
+        <v>0</v>
+      </c>
+      <c r="O510">
+        <v>0</v>
+      </c>
+      <c r="P510">
+        <v>20</v>
+      </c>
+      <c r="Q510">
+        <v>0</v>
+      </c>
+      <c r="R510">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="511" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>0</v>
+      </c>
+      <c r="B511" t="s">
+        <v>22</v>
+      </c>
+      <c r="C511" t="s">
+        <v>19</v>
+      </c>
+      <c r="D511" t="s">
+        <v>20</v>
+      </c>
+      <c r="E511">
+        <v>6144</v>
+      </c>
+      <c r="F511">
+        <v>3</v>
+      </c>
+      <c r="G511">
+        <v>0</v>
+      </c>
+      <c r="H511">
+        <v>1</v>
+      </c>
+      <c r="I511">
+        <v>0</v>
+      </c>
+      <c r="J511">
+        <v>0</v>
+      </c>
+      <c r="K511">
+        <v>0</v>
+      </c>
+      <c r="L511">
+        <v>0</v>
+      </c>
+      <c r="M511">
+        <v>12</v>
+      </c>
+      <c r="N511">
+        <v>0</v>
+      </c>
+      <c r="O511">
+        <v>0</v>
+      </c>
+      <c r="P511">
+        <v>16</v>
+      </c>
+      <c r="Q511">
+        <v>0</v>
+      </c>
+      <c r="R511">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="512" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>0</v>
+      </c>
+      <c r="B512" t="s">
+        <v>22</v>
+      </c>
+      <c r="C512" t="s">
+        <v>19</v>
+      </c>
+      <c r="D512" t="s">
+        <v>20</v>
+      </c>
+      <c r="E512">
+        <v>6144</v>
+      </c>
+      <c r="F512">
+        <v>4</v>
+      </c>
+      <c r="G512">
+        <v>0</v>
+      </c>
+      <c r="H512">
+        <v>3</v>
+      </c>
+      <c r="I512">
+        <v>0</v>
+      </c>
+      <c r="J512">
+        <v>0</v>
+      </c>
+      <c r="K512">
+        <v>0</v>
+      </c>
+      <c r="L512">
+        <v>0</v>
+      </c>
+      <c r="M512">
+        <v>104</v>
+      </c>
+      <c r="N512">
+        <v>162</v>
+      </c>
+      <c r="O512">
+        <v>0</v>
+      </c>
+      <c r="P512">
+        <v>273</v>
+      </c>
+      <c r="Q512">
+        <v>184</v>
+      </c>
+      <c r="R512">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="513" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>0</v>
+      </c>
+      <c r="B513" t="s">
+        <v>22</v>
+      </c>
+      <c r="C513" t="s">
+        <v>19</v>
+      </c>
+      <c r="D513" t="s">
+        <v>20</v>
+      </c>
+      <c r="E513">
+        <v>6144</v>
+      </c>
+      <c r="F513">
+        <v>4</v>
+      </c>
+      <c r="G513">
+        <v>0</v>
+      </c>
+      <c r="H513">
+        <v>1</v>
+      </c>
+      <c r="I513">
+        <v>1</v>
+      </c>
+      <c r="J513">
+        <v>0</v>
+      </c>
+      <c r="K513">
+        <v>0</v>
+      </c>
+      <c r="L513">
+        <v>0</v>
+      </c>
+      <c r="M513">
+        <v>22</v>
+      </c>
+      <c r="N513">
+        <v>2</v>
+      </c>
+      <c r="O513">
+        <v>0</v>
+      </c>
+      <c r="P513">
+        <v>30</v>
+      </c>
+      <c r="Q513">
+        <v>0</v>
+      </c>
+      <c r="R513">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="514" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>0</v>
+      </c>
+      <c r="B514" t="s">
+        <v>22</v>
+      </c>
+      <c r="C514" t="s">
+        <v>19</v>
+      </c>
+      <c r="D514" t="s">
+        <v>20</v>
+      </c>
+      <c r="E514">
+        <v>6144</v>
+      </c>
+      <c r="F514">
+        <v>3</v>
+      </c>
+      <c r="G514">
+        <v>0</v>
+      </c>
+      <c r="H514">
+        <v>2</v>
+      </c>
+      <c r="I514">
+        <v>0</v>
+      </c>
+      <c r="J514">
+        <v>0</v>
+      </c>
+      <c r="K514">
+        <v>0</v>
+      </c>
+      <c r="L514">
+        <v>0</v>
+      </c>
+      <c r="M514">
+        <v>13</v>
+      </c>
+      <c r="N514">
+        <v>2</v>
+      </c>
+      <c r="O514">
+        <v>0</v>
+      </c>
+      <c r="P514">
+        <v>20</v>
+      </c>
+      <c r="Q514">
+        <v>0</v>
+      </c>
+      <c r="R514">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="515" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>0</v>
+      </c>
+      <c r="B515" t="s">
+        <v>22</v>
+      </c>
+      <c r="C515" t="s">
+        <v>19</v>
+      </c>
+      <c r="D515" t="s">
+        <v>20</v>
+      </c>
+      <c r="E515">
+        <v>6144</v>
+      </c>
+      <c r="F515">
+        <v>4</v>
+      </c>
+      <c r="G515">
+        <v>0</v>
+      </c>
+      <c r="H515">
+        <v>4</v>
+      </c>
+      <c r="I515">
+        <v>1</v>
+      </c>
+      <c r="J515">
+        <v>0</v>
+      </c>
+      <c r="K515">
+        <v>0</v>
+      </c>
+      <c r="L515">
+        <v>0</v>
+      </c>
+      <c r="M515">
+        <v>17</v>
+      </c>
+      <c r="N515">
+        <v>6</v>
+      </c>
+      <c r="O515">
+        <v>0</v>
+      </c>
+      <c r="P515">
+        <v>32</v>
+      </c>
+      <c r="Q515">
+        <v>0</v>
+      </c>
+      <c r="R515">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="516" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>0</v>
+      </c>
+      <c r="B516" t="s">
+        <v>22</v>
+      </c>
+      <c r="C516" t="s">
+        <v>19</v>
+      </c>
+      <c r="D516" t="s">
+        <v>20</v>
+      </c>
+      <c r="E516">
+        <v>6144</v>
+      </c>
+      <c r="F516">
+        <v>5</v>
+      </c>
+      <c r="G516">
+        <v>0</v>
+      </c>
+      <c r="H516">
+        <v>1</v>
+      </c>
+      <c r="I516">
+        <v>0</v>
+      </c>
+      <c r="J516">
+        <v>0</v>
+      </c>
+      <c r="K516">
+        <v>0</v>
+      </c>
+      <c r="L516">
+        <v>0</v>
+      </c>
+      <c r="M516">
+        <v>18</v>
+      </c>
+      <c r="N516">
+        <v>3</v>
+      </c>
+      <c r="O516">
+        <v>0</v>
+      </c>
+      <c r="P516">
+        <v>27</v>
+      </c>
+      <c r="Q516">
+        <v>0</v>
+      </c>
+      <c r="R516">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="517" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>0</v>
+      </c>
+      <c r="B517" t="s">
+        <v>22</v>
+      </c>
+      <c r="C517" t="s">
+        <v>19</v>
+      </c>
+      <c r="D517" t="s">
+        <v>20</v>
+      </c>
+      <c r="E517">
+        <v>6144</v>
+      </c>
+      <c r="F517">
+        <v>3</v>
+      </c>
+      <c r="G517">
+        <v>0</v>
+      </c>
+      <c r="H517">
+        <v>2</v>
+      </c>
+      <c r="I517">
+        <v>0</v>
+      </c>
+      <c r="J517">
+        <v>0</v>
+      </c>
+      <c r="K517">
+        <v>0</v>
+      </c>
+      <c r="L517">
+        <v>0</v>
+      </c>
+      <c r="M517">
+        <v>21</v>
+      </c>
+      <c r="N517">
+        <v>2</v>
+      </c>
+      <c r="O517">
+        <v>0</v>
+      </c>
+      <c r="P517">
+        <v>28</v>
+      </c>
+      <c r="Q517">
+        <v>0</v>
+      </c>
+      <c r="R517">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="518" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>0</v>
+      </c>
+      <c r="B518" t="s">
+        <v>22</v>
+      </c>
+      <c r="C518" t="s">
+        <v>19</v>
+      </c>
+      <c r="D518" t="s">
+        <v>20</v>
+      </c>
+      <c r="E518">
+        <v>6144</v>
+      </c>
+      <c r="F518">
+        <v>5</v>
+      </c>
+      <c r="G518">
+        <v>0</v>
+      </c>
+      <c r="H518">
+        <v>2</v>
+      </c>
+      <c r="I518">
+        <v>0</v>
+      </c>
+      <c r="J518">
+        <v>0</v>
+      </c>
+      <c r="K518">
+        <v>0</v>
+      </c>
+      <c r="L518">
+        <v>0</v>
+      </c>
+      <c r="M518">
+        <v>14</v>
+      </c>
+      <c r="N518">
+        <v>4</v>
+      </c>
+      <c r="O518">
+        <v>0</v>
+      </c>
+      <c r="P518">
+        <v>25</v>
+      </c>
+      <c r="Q518">
+        <v>0</v>
+      </c>
+      <c r="R518">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="519" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>0</v>
+      </c>
+      <c r="B519" t="s">
+        <v>22</v>
+      </c>
+      <c r="C519" t="s">
+        <v>19</v>
+      </c>
+      <c r="D519" t="s">
+        <v>20</v>
+      </c>
+      <c r="E519">
+        <v>6144</v>
+      </c>
+      <c r="F519">
+        <v>4</v>
+      </c>
+      <c r="G519">
+        <v>0</v>
+      </c>
+      <c r="H519">
+        <v>1</v>
+      </c>
+      <c r="I519">
+        <v>0</v>
+      </c>
+      <c r="J519">
+        <v>0</v>
+      </c>
+      <c r="K519">
+        <v>0</v>
+      </c>
+      <c r="L519">
+        <v>0</v>
+      </c>
+      <c r="M519">
+        <v>12</v>
+      </c>
+      <c r="N519">
+        <v>3</v>
+      </c>
+      <c r="O519">
+        <v>0</v>
+      </c>
+      <c r="P519">
+        <v>20</v>
+      </c>
+      <c r="Q519">
+        <v>0</v>
+      </c>
+      <c r="R519">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="520" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>0</v>
+      </c>
+      <c r="B520" t="s">
+        <v>22</v>
+      </c>
+      <c r="C520" t="s">
+        <v>19</v>
+      </c>
+      <c r="D520" t="s">
+        <v>20</v>
+      </c>
+      <c r="E520">
+        <v>6144</v>
+      </c>
+      <c r="F520">
+        <v>5</v>
+      </c>
+      <c r="G520">
+        <v>0</v>
+      </c>
+      <c r="H520">
+        <v>1</v>
+      </c>
+      <c r="I520">
+        <v>0</v>
+      </c>
+      <c r="J520">
+        <v>0</v>
+      </c>
+      <c r="K520">
+        <v>0</v>
+      </c>
+      <c r="L520">
+        <v>0</v>
+      </c>
+      <c r="M520">
+        <v>14</v>
+      </c>
+      <c r="N520">
+        <v>3</v>
+      </c>
+      <c r="O520">
+        <v>0</v>
+      </c>
+      <c r="P520">
+        <v>23</v>
+      </c>
+      <c r="Q520">
+        <v>0</v>
+      </c>
+      <c r="R520">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Reduce console spam; don't save png by default.
</commit_message>
<xml_diff>
--- a/test-apps/testbed/frontend/performance/performanceResults.xlsx
+++ b/test-apps/testbed/frontend/performance/performanceResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="23">
   <si>
     <t/>
   </si>
@@ -459,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R541"/>
+  <dimension ref="A1:R583"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H25" sqref="H25"/>
@@ -30538,6 +30538,2340 @@
         <v>16</v>
       </c>
     </row>
+    <row r="542" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>0</v>
+      </c>
+      <c r="B542" t="s">
+        <v>22</v>
+      </c>
+      <c r="C542" t="s">
+        <v>19</v>
+      </c>
+      <c r="D542" t="s">
+        <v>20</v>
+      </c>
+      <c r="E542">
+        <v>102013</v>
+      </c>
+      <c r="F542">
+        <v>3</v>
+      </c>
+      <c r="G542">
+        <v>1</v>
+      </c>
+      <c r="H542">
+        <v>2</v>
+      </c>
+      <c r="I542">
+        <v>0</v>
+      </c>
+      <c r="J542">
+        <v>0</v>
+      </c>
+      <c r="K542">
+        <v>0</v>
+      </c>
+      <c r="L542">
+        <v>0</v>
+      </c>
+      <c r="M542">
+        <v>18</v>
+      </c>
+      <c r="N542">
+        <v>3</v>
+      </c>
+      <c r="O542">
+        <v>0</v>
+      </c>
+      <c r="P542">
+        <v>27</v>
+      </c>
+      <c r="Q542">
+        <v>1</v>
+      </c>
+      <c r="R542">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="543" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>0</v>
+      </c>
+      <c r="B543" t="s">
+        <v>22</v>
+      </c>
+      <c r="C543" t="s">
+        <v>19</v>
+      </c>
+      <c r="D543" t="s">
+        <v>20</v>
+      </c>
+      <c r="E543">
+        <v>102013</v>
+      </c>
+      <c r="F543">
+        <v>3</v>
+      </c>
+      <c r="G543">
+        <v>0</v>
+      </c>
+      <c r="H543">
+        <v>2</v>
+      </c>
+      <c r="I543">
+        <v>0</v>
+      </c>
+      <c r="J543">
+        <v>0</v>
+      </c>
+      <c r="K543">
+        <v>0</v>
+      </c>
+      <c r="L543">
+        <v>0</v>
+      </c>
+      <c r="M543">
+        <v>16</v>
+      </c>
+      <c r="N543">
+        <v>2</v>
+      </c>
+      <c r="O543">
+        <v>0</v>
+      </c>
+      <c r="P543">
+        <v>23</v>
+      </c>
+      <c r="Q543">
+        <v>0</v>
+      </c>
+      <c r="R543">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="544" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>0</v>
+      </c>
+      <c r="B544" t="s">
+        <v>22</v>
+      </c>
+      <c r="C544" t="s">
+        <v>19</v>
+      </c>
+      <c r="D544" t="s">
+        <v>20</v>
+      </c>
+      <c r="E544">
+        <v>102013</v>
+      </c>
+      <c r="F544">
+        <v>7</v>
+      </c>
+      <c r="G544">
+        <v>0</v>
+      </c>
+      <c r="H544">
+        <v>3</v>
+      </c>
+      <c r="I544">
+        <v>0</v>
+      </c>
+      <c r="J544">
+        <v>0</v>
+      </c>
+      <c r="K544">
+        <v>0</v>
+      </c>
+      <c r="L544">
+        <v>0</v>
+      </c>
+      <c r="M544">
+        <v>30</v>
+      </c>
+      <c r="N544">
+        <v>3</v>
+      </c>
+      <c r="O544">
+        <v>0</v>
+      </c>
+      <c r="P544">
+        <v>43</v>
+      </c>
+      <c r="Q544">
+        <v>0</v>
+      </c>
+      <c r="R544">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="545" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>0</v>
+      </c>
+      <c r="B545" t="s">
+        <v>22</v>
+      </c>
+      <c r="C545" t="s">
+        <v>19</v>
+      </c>
+      <c r="D545" t="s">
+        <v>20</v>
+      </c>
+      <c r="E545">
+        <v>102013</v>
+      </c>
+      <c r="F545">
+        <v>1</v>
+      </c>
+      <c r="G545">
+        <v>0</v>
+      </c>
+      <c r="H545">
+        <v>1</v>
+      </c>
+      <c r="I545">
+        <v>0</v>
+      </c>
+      <c r="J545">
+        <v>0</v>
+      </c>
+      <c r="K545">
+        <v>0</v>
+      </c>
+      <c r="L545">
+        <v>0</v>
+      </c>
+      <c r="M545">
+        <v>12</v>
+      </c>
+      <c r="N545">
+        <v>2</v>
+      </c>
+      <c r="O545">
+        <v>0</v>
+      </c>
+      <c r="P545">
+        <v>16</v>
+      </c>
+      <c r="Q545">
+        <v>0</v>
+      </c>
+      <c r="R545">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="546" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>0</v>
+      </c>
+      <c r="B546" t="s">
+        <v>22</v>
+      </c>
+      <c r="C546" t="s">
+        <v>19</v>
+      </c>
+      <c r="D546" t="s">
+        <v>20</v>
+      </c>
+      <c r="E546">
+        <v>102013</v>
+      </c>
+      <c r="F546">
+        <v>2</v>
+      </c>
+      <c r="G546">
+        <v>0</v>
+      </c>
+      <c r="H546">
+        <v>2</v>
+      </c>
+      <c r="I546">
+        <v>1</v>
+      </c>
+      <c r="J546">
+        <v>0</v>
+      </c>
+      <c r="K546">
+        <v>0</v>
+      </c>
+      <c r="L546">
+        <v>0</v>
+      </c>
+      <c r="M546">
+        <v>23</v>
+      </c>
+      <c r="N546">
+        <v>3</v>
+      </c>
+      <c r="O546">
+        <v>0</v>
+      </c>
+      <c r="P546">
+        <v>31</v>
+      </c>
+      <c r="Q546">
+        <v>0</v>
+      </c>
+      <c r="R546">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="547" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>0</v>
+      </c>
+      <c r="B547" t="s">
+        <v>22</v>
+      </c>
+      <c r="C547" t="s">
+        <v>19</v>
+      </c>
+      <c r="D547" t="s">
+        <v>20</v>
+      </c>
+      <c r="E547">
+        <v>102013</v>
+      </c>
+      <c r="F547">
+        <v>3</v>
+      </c>
+      <c r="G547">
+        <v>0</v>
+      </c>
+      <c r="H547">
+        <v>2</v>
+      </c>
+      <c r="I547">
+        <v>0</v>
+      </c>
+      <c r="J547">
+        <v>0</v>
+      </c>
+      <c r="K547">
+        <v>0</v>
+      </c>
+      <c r="L547">
+        <v>0</v>
+      </c>
+      <c r="M547">
+        <v>19</v>
+      </c>
+      <c r="N547">
+        <v>2</v>
+      </c>
+      <c r="O547">
+        <v>0</v>
+      </c>
+      <c r="P547">
+        <v>26</v>
+      </c>
+      <c r="Q547">
+        <v>0</v>
+      </c>
+      <c r="R547">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="548" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>0</v>
+      </c>
+      <c r="B548" t="s">
+        <v>22</v>
+      </c>
+      <c r="C548" t="s">
+        <v>19</v>
+      </c>
+      <c r="D548" t="s">
+        <v>20</v>
+      </c>
+      <c r="E548">
+        <v>102013</v>
+      </c>
+      <c r="F548">
+        <v>3</v>
+      </c>
+      <c r="G548">
+        <v>0</v>
+      </c>
+      <c r="H548">
+        <v>3</v>
+      </c>
+      <c r="I548">
+        <v>0</v>
+      </c>
+      <c r="J548">
+        <v>0</v>
+      </c>
+      <c r="K548">
+        <v>0</v>
+      </c>
+      <c r="L548">
+        <v>0</v>
+      </c>
+      <c r="M548">
+        <v>22</v>
+      </c>
+      <c r="N548">
+        <v>2</v>
+      </c>
+      <c r="O548">
+        <v>0</v>
+      </c>
+      <c r="P548">
+        <v>30</v>
+      </c>
+      <c r="Q548">
+        <v>0</v>
+      </c>
+      <c r="R548">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="549" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>0</v>
+      </c>
+      <c r="B549" t="s">
+        <v>22</v>
+      </c>
+      <c r="C549" t="s">
+        <v>19</v>
+      </c>
+      <c r="D549" t="s">
+        <v>20</v>
+      </c>
+      <c r="E549">
+        <v>102013</v>
+      </c>
+      <c r="F549">
+        <v>5</v>
+      </c>
+      <c r="G549">
+        <v>1</v>
+      </c>
+      <c r="H549">
+        <v>1</v>
+      </c>
+      <c r="I549">
+        <v>1</v>
+      </c>
+      <c r="J549">
+        <v>0</v>
+      </c>
+      <c r="K549">
+        <v>0</v>
+      </c>
+      <c r="L549">
+        <v>0</v>
+      </c>
+      <c r="M549">
+        <v>17</v>
+      </c>
+      <c r="N549">
+        <v>3</v>
+      </c>
+      <c r="O549">
+        <v>0</v>
+      </c>
+      <c r="P549">
+        <v>28</v>
+      </c>
+      <c r="Q549">
+        <v>0</v>
+      </c>
+      <c r="R549">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="550" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>0</v>
+      </c>
+      <c r="B550" t="s">
+        <v>22</v>
+      </c>
+      <c r="C550" t="s">
+        <v>19</v>
+      </c>
+      <c r="D550" t="s">
+        <v>20</v>
+      </c>
+      <c r="E550">
+        <v>102013</v>
+      </c>
+      <c r="F550">
+        <v>2</v>
+      </c>
+      <c r="G550">
+        <v>0</v>
+      </c>
+      <c r="H550">
+        <v>2</v>
+      </c>
+      <c r="I550">
+        <v>0</v>
+      </c>
+      <c r="J550">
+        <v>0</v>
+      </c>
+      <c r="K550">
+        <v>0</v>
+      </c>
+      <c r="L550">
+        <v>0</v>
+      </c>
+      <c r="M550">
+        <v>19</v>
+      </c>
+      <c r="N550">
+        <v>2</v>
+      </c>
+      <c r="O550">
+        <v>0</v>
+      </c>
+      <c r="P550">
+        <v>25</v>
+      </c>
+      <c r="Q550">
+        <v>0</v>
+      </c>
+      <c r="R550">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="551" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>0</v>
+      </c>
+      <c r="B551" t="s">
+        <v>22</v>
+      </c>
+      <c r="C551" t="s">
+        <v>19</v>
+      </c>
+      <c r="D551" t="s">
+        <v>20</v>
+      </c>
+      <c r="E551">
+        <v>102013</v>
+      </c>
+      <c r="F551">
+        <v>2</v>
+      </c>
+      <c r="G551">
+        <v>0</v>
+      </c>
+      <c r="H551">
+        <v>1</v>
+      </c>
+      <c r="I551">
+        <v>0</v>
+      </c>
+      <c r="J551">
+        <v>0</v>
+      </c>
+      <c r="K551">
+        <v>0</v>
+      </c>
+      <c r="L551">
+        <v>0</v>
+      </c>
+      <c r="M551">
+        <v>11</v>
+      </c>
+      <c r="N551">
+        <v>2</v>
+      </c>
+      <c r="O551">
+        <v>0</v>
+      </c>
+      <c r="P551">
+        <v>16</v>
+      </c>
+      <c r="Q551">
+        <v>0</v>
+      </c>
+      <c r="R551">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="552" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>0</v>
+      </c>
+      <c r="B552" t="s">
+        <v>22</v>
+      </c>
+      <c r="C552" t="s">
+        <v>19</v>
+      </c>
+      <c r="D552" t="s">
+        <v>20</v>
+      </c>
+      <c r="E552">
+        <v>102013</v>
+      </c>
+      <c r="F552">
+        <v>2</v>
+      </c>
+      <c r="G552">
+        <v>0</v>
+      </c>
+      <c r="H552">
+        <v>3</v>
+      </c>
+      <c r="I552">
+        <v>0</v>
+      </c>
+      <c r="J552">
+        <v>0</v>
+      </c>
+      <c r="K552">
+        <v>0</v>
+      </c>
+      <c r="L552">
+        <v>0</v>
+      </c>
+      <c r="M552">
+        <v>11</v>
+      </c>
+      <c r="N552">
+        <v>1</v>
+      </c>
+      <c r="O552">
+        <v>0</v>
+      </c>
+      <c r="P552">
+        <v>17</v>
+      </c>
+      <c r="Q552">
+        <v>0</v>
+      </c>
+      <c r="R552">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="553" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" t="s">
+        <v>22</v>
+      </c>
+      <c r="C553" t="s">
+        <v>19</v>
+      </c>
+      <c r="D553" t="s">
+        <v>20</v>
+      </c>
+      <c r="E553">
+        <v>102013</v>
+      </c>
+      <c r="F553">
+        <v>2</v>
+      </c>
+      <c r="G553">
+        <v>0</v>
+      </c>
+      <c r="H553">
+        <v>2</v>
+      </c>
+      <c r="I553">
+        <v>0</v>
+      </c>
+      <c r="J553">
+        <v>0</v>
+      </c>
+      <c r="K553">
+        <v>0</v>
+      </c>
+      <c r="L553">
+        <v>0</v>
+      </c>
+      <c r="M553">
+        <v>19</v>
+      </c>
+      <c r="N553">
+        <v>2</v>
+      </c>
+      <c r="O553">
+        <v>0</v>
+      </c>
+      <c r="P553">
+        <v>25</v>
+      </c>
+      <c r="Q553">
+        <v>0</v>
+      </c>
+      <c r="R553">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="554" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>0</v>
+      </c>
+      <c r="B554" t="s">
+        <v>22</v>
+      </c>
+      <c r="C554" t="s">
+        <v>19</v>
+      </c>
+      <c r="D554" t="s">
+        <v>20</v>
+      </c>
+      <c r="E554">
+        <v>102013</v>
+      </c>
+      <c r="F554">
+        <v>2</v>
+      </c>
+      <c r="G554">
+        <v>0</v>
+      </c>
+      <c r="H554">
+        <v>5</v>
+      </c>
+      <c r="I554">
+        <v>0</v>
+      </c>
+      <c r="J554">
+        <v>0</v>
+      </c>
+      <c r="K554">
+        <v>0</v>
+      </c>
+      <c r="L554">
+        <v>0</v>
+      </c>
+      <c r="M554">
+        <v>19</v>
+      </c>
+      <c r="N554">
+        <v>2</v>
+      </c>
+      <c r="O554">
+        <v>0</v>
+      </c>
+      <c r="P554">
+        <v>28</v>
+      </c>
+      <c r="Q554">
+        <v>0</v>
+      </c>
+      <c r="R554">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="555" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>0</v>
+      </c>
+      <c r="B555" t="s">
+        <v>22</v>
+      </c>
+      <c r="C555" t="s">
+        <v>19</v>
+      </c>
+      <c r="D555" t="s">
+        <v>20</v>
+      </c>
+      <c r="E555">
+        <v>102013</v>
+      </c>
+      <c r="F555">
+        <v>2</v>
+      </c>
+      <c r="G555">
+        <v>0</v>
+      </c>
+      <c r="H555">
+        <v>1</v>
+      </c>
+      <c r="I555">
+        <v>1</v>
+      </c>
+      <c r="J555">
+        <v>0</v>
+      </c>
+      <c r="K555">
+        <v>0</v>
+      </c>
+      <c r="L555">
+        <v>0</v>
+      </c>
+      <c r="M555">
+        <v>19</v>
+      </c>
+      <c r="N555">
+        <v>2</v>
+      </c>
+      <c r="O555">
+        <v>0</v>
+      </c>
+      <c r="P555">
+        <v>25</v>
+      </c>
+      <c r="Q555">
+        <v>0</v>
+      </c>
+      <c r="R555">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="556" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>0</v>
+      </c>
+      <c r="B556" t="s">
+        <v>22</v>
+      </c>
+      <c r="C556" t="s">
+        <v>19</v>
+      </c>
+      <c r="D556" t="s">
+        <v>20</v>
+      </c>
+      <c r="E556">
+        <v>102013</v>
+      </c>
+      <c r="F556">
+        <v>1</v>
+      </c>
+      <c r="G556">
+        <v>0</v>
+      </c>
+      <c r="H556">
+        <v>2</v>
+      </c>
+      <c r="I556">
+        <v>1</v>
+      </c>
+      <c r="J556">
+        <v>0</v>
+      </c>
+      <c r="K556">
+        <v>0</v>
+      </c>
+      <c r="L556">
+        <v>0</v>
+      </c>
+      <c r="M556">
+        <v>11</v>
+      </c>
+      <c r="N556">
+        <v>1</v>
+      </c>
+      <c r="O556">
+        <v>0</v>
+      </c>
+      <c r="P556">
+        <v>16</v>
+      </c>
+      <c r="Q556">
+        <v>0</v>
+      </c>
+      <c r="R556">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="557" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>0</v>
+      </c>
+      <c r="B557" t="s">
+        <v>22</v>
+      </c>
+      <c r="C557" t="s">
+        <v>19</v>
+      </c>
+      <c r="D557" t="s">
+        <v>20</v>
+      </c>
+      <c r="E557">
+        <v>102013</v>
+      </c>
+      <c r="F557">
+        <v>6</v>
+      </c>
+      <c r="G557">
+        <v>0</v>
+      </c>
+      <c r="H557">
+        <v>2</v>
+      </c>
+      <c r="I557">
+        <v>0</v>
+      </c>
+      <c r="J557">
+        <v>0</v>
+      </c>
+      <c r="K557">
+        <v>0</v>
+      </c>
+      <c r="L557">
+        <v>0</v>
+      </c>
+      <c r="M557">
+        <v>10</v>
+      </c>
+      <c r="N557">
+        <v>2</v>
+      </c>
+      <c r="O557">
+        <v>0</v>
+      </c>
+      <c r="P557">
+        <v>20</v>
+      </c>
+      <c r="Q557">
+        <v>0</v>
+      </c>
+      <c r="R557">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="558" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>0</v>
+      </c>
+      <c r="B558" t="s">
+        <v>22</v>
+      </c>
+      <c r="C558" t="s">
+        <v>19</v>
+      </c>
+      <c r="D558" t="s">
+        <v>20</v>
+      </c>
+      <c r="E558">
+        <v>102013</v>
+      </c>
+      <c r="F558">
+        <v>2</v>
+      </c>
+      <c r="G558">
+        <v>0</v>
+      </c>
+      <c r="H558">
+        <v>1</v>
+      </c>
+      <c r="I558">
+        <v>1</v>
+      </c>
+      <c r="J558">
+        <v>0</v>
+      </c>
+      <c r="K558">
+        <v>0</v>
+      </c>
+      <c r="L558">
+        <v>0</v>
+      </c>
+      <c r="M558">
+        <v>19</v>
+      </c>
+      <c r="N558">
+        <v>4</v>
+      </c>
+      <c r="O558">
+        <v>0</v>
+      </c>
+      <c r="P558">
+        <v>27</v>
+      </c>
+      <c r="Q558">
+        <v>0</v>
+      </c>
+      <c r="R558">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="559" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>0</v>
+      </c>
+      <c r="B559" t="s">
+        <v>22</v>
+      </c>
+      <c r="C559" t="s">
+        <v>19</v>
+      </c>
+      <c r="D559" t="s">
+        <v>20</v>
+      </c>
+      <c r="E559">
+        <v>102013</v>
+      </c>
+      <c r="F559">
+        <v>2</v>
+      </c>
+      <c r="G559">
+        <v>0</v>
+      </c>
+      <c r="H559">
+        <v>1</v>
+      </c>
+      <c r="I559">
+        <v>0</v>
+      </c>
+      <c r="J559">
+        <v>0</v>
+      </c>
+      <c r="K559">
+        <v>0</v>
+      </c>
+      <c r="L559">
+        <v>0</v>
+      </c>
+      <c r="M559">
+        <v>9</v>
+      </c>
+      <c r="N559">
+        <v>3</v>
+      </c>
+      <c r="O559">
+        <v>0</v>
+      </c>
+      <c r="P559">
+        <v>15</v>
+      </c>
+      <c r="Q559">
+        <v>0</v>
+      </c>
+      <c r="R559">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="560" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>0</v>
+      </c>
+      <c r="B560" t="s">
+        <v>22</v>
+      </c>
+      <c r="C560" t="s">
+        <v>19</v>
+      </c>
+      <c r="D560" t="s">
+        <v>20</v>
+      </c>
+      <c r="E560">
+        <v>102013</v>
+      </c>
+      <c r="F560">
+        <v>2</v>
+      </c>
+      <c r="G560">
+        <v>0</v>
+      </c>
+      <c r="H560">
+        <v>1</v>
+      </c>
+      <c r="I560">
+        <v>1</v>
+      </c>
+      <c r="J560">
+        <v>0</v>
+      </c>
+      <c r="K560">
+        <v>0</v>
+      </c>
+      <c r="L560">
+        <v>0</v>
+      </c>
+      <c r="M560">
+        <v>9</v>
+      </c>
+      <c r="N560">
+        <v>1</v>
+      </c>
+      <c r="O560">
+        <v>1</v>
+      </c>
+      <c r="P560">
+        <v>15</v>
+      </c>
+      <c r="Q560">
+        <v>0</v>
+      </c>
+      <c r="R560">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="561" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>0</v>
+      </c>
+      <c r="B561" t="s">
+        <v>22</v>
+      </c>
+      <c r="C561" t="s">
+        <v>19</v>
+      </c>
+      <c r="D561" t="s">
+        <v>20</v>
+      </c>
+      <c r="E561">
+        <v>102013</v>
+      </c>
+      <c r="F561">
+        <v>1</v>
+      </c>
+      <c r="G561">
+        <v>0</v>
+      </c>
+      <c r="H561">
+        <v>1</v>
+      </c>
+      <c r="I561">
+        <v>0</v>
+      </c>
+      <c r="J561">
+        <v>0</v>
+      </c>
+      <c r="K561">
+        <v>0</v>
+      </c>
+      <c r="L561">
+        <v>0</v>
+      </c>
+      <c r="M561">
+        <v>11</v>
+      </c>
+      <c r="N561">
+        <v>2</v>
+      </c>
+      <c r="O561">
+        <v>0</v>
+      </c>
+      <c r="P561">
+        <v>15</v>
+      </c>
+      <c r="Q561">
+        <v>0</v>
+      </c>
+      <c r="R561">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="562" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D562" t="s">
+        <v>21</v>
+      </c>
+      <c r="E562">
+        <v>102013</v>
+      </c>
+      <c r="F562">
+        <v>1</v>
+      </c>
+      <c r="G562">
+        <v>0</v>
+      </c>
+      <c r="H562">
+        <v>1</v>
+      </c>
+      <c r="I562">
+        <v>0</v>
+      </c>
+      <c r="J562">
+        <v>0</v>
+      </c>
+      <c r="K562">
+        <v>0</v>
+      </c>
+      <c r="L562">
+        <v>0</v>
+      </c>
+      <c r="M562">
+        <v>11</v>
+      </c>
+      <c r="N562">
+        <v>2</v>
+      </c>
+      <c r="O562">
+        <v>0</v>
+      </c>
+      <c r="P562">
+        <v>15</v>
+      </c>
+      <c r="Q562">
+        <v>0</v>
+      </c>
+      <c r="R562">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="563" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>0</v>
+      </c>
+      <c r="B563" t="s">
+        <v>22</v>
+      </c>
+      <c r="C563" t="s">
+        <v>19</v>
+      </c>
+      <c r="D563" t="s">
+        <v>20</v>
+      </c>
+      <c r="E563">
+        <v>102486</v>
+      </c>
+      <c r="F563">
+        <v>3</v>
+      </c>
+      <c r="G563">
+        <v>1</v>
+      </c>
+      <c r="H563">
+        <v>2</v>
+      </c>
+      <c r="I563">
+        <v>1</v>
+      </c>
+      <c r="J563">
+        <v>0</v>
+      </c>
+      <c r="K563">
+        <v>0</v>
+      </c>
+      <c r="L563">
+        <v>0</v>
+      </c>
+      <c r="M563">
+        <v>35</v>
+      </c>
+      <c r="N563">
+        <v>4</v>
+      </c>
+      <c r="O563">
+        <v>0</v>
+      </c>
+      <c r="P563">
+        <v>46</v>
+      </c>
+      <c r="Q563">
+        <v>0</v>
+      </c>
+      <c r="R563">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="564" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>0</v>
+      </c>
+      <c r="B564" t="s">
+        <v>22</v>
+      </c>
+      <c r="C564" t="s">
+        <v>19</v>
+      </c>
+      <c r="D564" t="s">
+        <v>20</v>
+      </c>
+      <c r="E564">
+        <v>102486</v>
+      </c>
+      <c r="F564">
+        <v>10</v>
+      </c>
+      <c r="G564">
+        <v>0</v>
+      </c>
+      <c r="H564">
+        <v>5</v>
+      </c>
+      <c r="I564">
+        <v>0</v>
+      </c>
+      <c r="J564">
+        <v>0</v>
+      </c>
+      <c r="K564">
+        <v>0</v>
+      </c>
+      <c r="L564">
+        <v>0</v>
+      </c>
+      <c r="M564">
+        <v>19</v>
+      </c>
+      <c r="N564">
+        <v>3</v>
+      </c>
+      <c r="O564">
+        <v>0</v>
+      </c>
+      <c r="P564">
+        <v>37</v>
+      </c>
+      <c r="Q564">
+        <v>0</v>
+      </c>
+      <c r="R564">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="565" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>0</v>
+      </c>
+      <c r="B565" t="s">
+        <v>22</v>
+      </c>
+      <c r="C565" t="s">
+        <v>19</v>
+      </c>
+      <c r="D565" t="s">
+        <v>20</v>
+      </c>
+      <c r="E565">
+        <v>102486</v>
+      </c>
+      <c r="F565">
+        <v>3</v>
+      </c>
+      <c r="G565">
+        <v>0</v>
+      </c>
+      <c r="H565">
+        <v>1</v>
+      </c>
+      <c r="I565">
+        <v>1</v>
+      </c>
+      <c r="J565">
+        <v>0</v>
+      </c>
+      <c r="K565">
+        <v>0</v>
+      </c>
+      <c r="L565">
+        <v>0</v>
+      </c>
+      <c r="M565">
+        <v>25</v>
+      </c>
+      <c r="N565">
+        <v>3</v>
+      </c>
+      <c r="O565">
+        <v>0</v>
+      </c>
+      <c r="P565">
+        <v>33</v>
+      </c>
+      <c r="Q565">
+        <v>0</v>
+      </c>
+      <c r="R565">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="566" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>0</v>
+      </c>
+      <c r="B566" t="s">
+        <v>22</v>
+      </c>
+      <c r="C566" t="s">
+        <v>19</v>
+      </c>
+      <c r="D566" t="s">
+        <v>20</v>
+      </c>
+      <c r="E566">
+        <v>102486</v>
+      </c>
+      <c r="F566">
+        <v>2</v>
+      </c>
+      <c r="G566">
+        <v>0</v>
+      </c>
+      <c r="H566">
+        <v>2</v>
+      </c>
+      <c r="I566">
+        <v>0</v>
+      </c>
+      <c r="J566">
+        <v>0</v>
+      </c>
+      <c r="K566">
+        <v>0</v>
+      </c>
+      <c r="L566">
+        <v>0</v>
+      </c>
+      <c r="M566">
+        <v>23</v>
+      </c>
+      <c r="N566">
+        <v>3</v>
+      </c>
+      <c r="O566">
+        <v>0</v>
+      </c>
+      <c r="P566">
+        <v>30</v>
+      </c>
+      <c r="Q566">
+        <v>0</v>
+      </c>
+      <c r="R566">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="567" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>0</v>
+      </c>
+      <c r="B567" t="s">
+        <v>22</v>
+      </c>
+      <c r="C567" t="s">
+        <v>19</v>
+      </c>
+      <c r="D567" t="s">
+        <v>20</v>
+      </c>
+      <c r="E567">
+        <v>102486</v>
+      </c>
+      <c r="F567">
+        <v>4</v>
+      </c>
+      <c r="G567">
+        <v>0</v>
+      </c>
+      <c r="H567">
+        <v>2</v>
+      </c>
+      <c r="I567">
+        <v>0</v>
+      </c>
+      <c r="J567">
+        <v>0</v>
+      </c>
+      <c r="K567">
+        <v>0</v>
+      </c>
+      <c r="L567">
+        <v>0</v>
+      </c>
+      <c r="M567">
+        <v>19</v>
+      </c>
+      <c r="N567">
+        <v>3</v>
+      </c>
+      <c r="O567">
+        <v>0</v>
+      </c>
+      <c r="P567">
+        <v>28</v>
+      </c>
+      <c r="Q567">
+        <v>0</v>
+      </c>
+      <c r="R567">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="568" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>0</v>
+      </c>
+      <c r="B568" t="s">
+        <v>22</v>
+      </c>
+      <c r="C568" t="s">
+        <v>19</v>
+      </c>
+      <c r="D568" t="s">
+        <v>20</v>
+      </c>
+      <c r="E568">
+        <v>102486</v>
+      </c>
+      <c r="F568">
+        <v>2</v>
+      </c>
+      <c r="G568">
+        <v>0</v>
+      </c>
+      <c r="H568">
+        <v>2</v>
+      </c>
+      <c r="I568">
+        <v>0</v>
+      </c>
+      <c r="J568">
+        <v>0</v>
+      </c>
+      <c r="K568">
+        <v>0</v>
+      </c>
+      <c r="L568">
+        <v>0</v>
+      </c>
+      <c r="M568">
+        <v>18</v>
+      </c>
+      <c r="N568">
+        <v>3</v>
+      </c>
+      <c r="O568">
+        <v>0</v>
+      </c>
+      <c r="P568">
+        <v>25</v>
+      </c>
+      <c r="Q568">
+        <v>0</v>
+      </c>
+      <c r="R568">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="569" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>0</v>
+      </c>
+      <c r="B569" t="s">
+        <v>22</v>
+      </c>
+      <c r="C569" t="s">
+        <v>19</v>
+      </c>
+      <c r="D569" t="s">
+        <v>20</v>
+      </c>
+      <c r="E569">
+        <v>102486</v>
+      </c>
+      <c r="F569">
+        <v>2</v>
+      </c>
+      <c r="G569">
+        <v>0</v>
+      </c>
+      <c r="H569">
+        <v>2</v>
+      </c>
+      <c r="I569">
+        <v>1</v>
+      </c>
+      <c r="J569">
+        <v>0</v>
+      </c>
+      <c r="K569">
+        <v>0</v>
+      </c>
+      <c r="L569">
+        <v>0</v>
+      </c>
+      <c r="M569">
+        <v>15</v>
+      </c>
+      <c r="N569">
+        <v>2</v>
+      </c>
+      <c r="O569">
+        <v>0</v>
+      </c>
+      <c r="P569">
+        <v>22</v>
+      </c>
+      <c r="Q569">
+        <v>0</v>
+      </c>
+      <c r="R569">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="570" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>0</v>
+      </c>
+      <c r="B570" t="s">
+        <v>22</v>
+      </c>
+      <c r="C570" t="s">
+        <v>19</v>
+      </c>
+      <c r="D570" t="s">
+        <v>20</v>
+      </c>
+      <c r="E570">
+        <v>102486</v>
+      </c>
+      <c r="F570">
+        <v>4</v>
+      </c>
+      <c r="G570">
+        <v>0</v>
+      </c>
+      <c r="H570">
+        <v>2</v>
+      </c>
+      <c r="I570">
+        <v>0</v>
+      </c>
+      <c r="J570">
+        <v>0</v>
+      </c>
+      <c r="K570">
+        <v>0</v>
+      </c>
+      <c r="L570">
+        <v>0</v>
+      </c>
+      <c r="M570">
+        <v>17</v>
+      </c>
+      <c r="N570">
+        <v>2</v>
+      </c>
+      <c r="O570">
+        <v>0</v>
+      </c>
+      <c r="P570">
+        <v>25</v>
+      </c>
+      <c r="Q570">
+        <v>0</v>
+      </c>
+      <c r="R570">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="571" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>0</v>
+      </c>
+      <c r="B571" t="s">
+        <v>22</v>
+      </c>
+      <c r="C571" t="s">
+        <v>19</v>
+      </c>
+      <c r="D571" t="s">
+        <v>20</v>
+      </c>
+      <c r="E571">
+        <v>102486</v>
+      </c>
+      <c r="F571">
+        <v>3</v>
+      </c>
+      <c r="G571">
+        <v>0</v>
+      </c>
+      <c r="H571">
+        <v>1</v>
+      </c>
+      <c r="I571">
+        <v>0</v>
+      </c>
+      <c r="J571">
+        <v>0</v>
+      </c>
+      <c r="K571">
+        <v>0</v>
+      </c>
+      <c r="L571">
+        <v>0</v>
+      </c>
+      <c r="M571">
+        <v>16</v>
+      </c>
+      <c r="N571">
+        <v>1</v>
+      </c>
+      <c r="O571">
+        <v>0</v>
+      </c>
+      <c r="P571">
+        <v>21</v>
+      </c>
+      <c r="Q571">
+        <v>0</v>
+      </c>
+      <c r="R571">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="572" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>0</v>
+      </c>
+      <c r="B572" t="s">
+        <v>22</v>
+      </c>
+      <c r="C572" t="s">
+        <v>19</v>
+      </c>
+      <c r="D572" t="s">
+        <v>20</v>
+      </c>
+      <c r="E572">
+        <v>102486</v>
+      </c>
+      <c r="F572">
+        <v>2</v>
+      </c>
+      <c r="G572">
+        <v>0</v>
+      </c>
+      <c r="H572">
+        <v>2</v>
+      </c>
+      <c r="I572">
+        <v>0</v>
+      </c>
+      <c r="J572">
+        <v>0</v>
+      </c>
+      <c r="K572">
+        <v>0</v>
+      </c>
+      <c r="L572">
+        <v>0</v>
+      </c>
+      <c r="M572">
+        <v>13</v>
+      </c>
+      <c r="N572">
+        <v>3</v>
+      </c>
+      <c r="O572">
+        <v>0</v>
+      </c>
+      <c r="P572">
+        <v>20</v>
+      </c>
+      <c r="Q572">
+        <v>0</v>
+      </c>
+      <c r="R572">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="573" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>0</v>
+      </c>
+      <c r="B573" t="s">
+        <v>22</v>
+      </c>
+      <c r="C573" t="s">
+        <v>19</v>
+      </c>
+      <c r="D573" t="s">
+        <v>20</v>
+      </c>
+      <c r="E573">
+        <v>102486</v>
+      </c>
+      <c r="F573">
+        <v>4</v>
+      </c>
+      <c r="G573">
+        <v>0</v>
+      </c>
+      <c r="H573">
+        <v>2</v>
+      </c>
+      <c r="I573">
+        <v>0</v>
+      </c>
+      <c r="J573">
+        <v>0</v>
+      </c>
+      <c r="K573">
+        <v>0</v>
+      </c>
+      <c r="L573">
+        <v>0</v>
+      </c>
+      <c r="M573">
+        <v>14</v>
+      </c>
+      <c r="N573">
+        <v>2</v>
+      </c>
+      <c r="O573">
+        <v>0</v>
+      </c>
+      <c r="P573">
+        <v>22</v>
+      </c>
+      <c r="Q573">
+        <v>0</v>
+      </c>
+      <c r="R573">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="574" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>0</v>
+      </c>
+      <c r="B574" t="s">
+        <v>22</v>
+      </c>
+      <c r="C574" t="s">
+        <v>19</v>
+      </c>
+      <c r="D574" t="s">
+        <v>20</v>
+      </c>
+      <c r="E574">
+        <v>102486</v>
+      </c>
+      <c r="F574">
+        <v>2</v>
+      </c>
+      <c r="G574">
+        <v>0</v>
+      </c>
+      <c r="H574">
+        <v>2</v>
+      </c>
+      <c r="I574">
+        <v>0</v>
+      </c>
+      <c r="J574">
+        <v>0</v>
+      </c>
+      <c r="K574">
+        <v>0</v>
+      </c>
+      <c r="L574">
+        <v>0</v>
+      </c>
+      <c r="M574">
+        <v>15</v>
+      </c>
+      <c r="N574">
+        <v>3</v>
+      </c>
+      <c r="O574">
+        <v>0</v>
+      </c>
+      <c r="P574">
+        <v>22</v>
+      </c>
+      <c r="Q574">
+        <v>0</v>
+      </c>
+      <c r="R574">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="575" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>0</v>
+      </c>
+      <c r="B575" t="s">
+        <v>22</v>
+      </c>
+      <c r="C575" t="s">
+        <v>19</v>
+      </c>
+      <c r="D575" t="s">
+        <v>20</v>
+      </c>
+      <c r="E575">
+        <v>102486</v>
+      </c>
+      <c r="F575">
+        <v>2</v>
+      </c>
+      <c r="G575">
+        <v>0</v>
+      </c>
+      <c r="H575">
+        <v>2</v>
+      </c>
+      <c r="I575">
+        <v>0</v>
+      </c>
+      <c r="J575">
+        <v>0</v>
+      </c>
+      <c r="K575">
+        <v>0</v>
+      </c>
+      <c r="L575">
+        <v>0</v>
+      </c>
+      <c r="M575">
+        <v>15</v>
+      </c>
+      <c r="N575">
+        <v>2</v>
+      </c>
+      <c r="O575">
+        <v>0</v>
+      </c>
+      <c r="P575">
+        <v>21</v>
+      </c>
+      <c r="Q575">
+        <v>0</v>
+      </c>
+      <c r="R575">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="576" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>0</v>
+      </c>
+      <c r="B576" t="s">
+        <v>22</v>
+      </c>
+      <c r="C576" t="s">
+        <v>19</v>
+      </c>
+      <c r="D576" t="s">
+        <v>20</v>
+      </c>
+      <c r="E576">
+        <v>102486</v>
+      </c>
+      <c r="F576">
+        <v>2</v>
+      </c>
+      <c r="G576">
+        <v>1</v>
+      </c>
+      <c r="H576">
+        <v>2</v>
+      </c>
+      <c r="I576">
+        <v>1</v>
+      </c>
+      <c r="J576">
+        <v>0</v>
+      </c>
+      <c r="K576">
+        <v>0</v>
+      </c>
+      <c r="L576">
+        <v>0</v>
+      </c>
+      <c r="M576">
+        <v>18</v>
+      </c>
+      <c r="N576">
+        <v>4</v>
+      </c>
+      <c r="O576">
+        <v>0</v>
+      </c>
+      <c r="P576">
+        <v>28</v>
+      </c>
+      <c r="Q576">
+        <v>0</v>
+      </c>
+      <c r="R576">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="577" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>0</v>
+      </c>
+      <c r="B577" t="s">
+        <v>22</v>
+      </c>
+      <c r="C577" t="s">
+        <v>19</v>
+      </c>
+      <c r="D577" t="s">
+        <v>20</v>
+      </c>
+      <c r="E577">
+        <v>102486</v>
+      </c>
+      <c r="F577">
+        <v>2</v>
+      </c>
+      <c r="G577">
+        <v>0</v>
+      </c>
+      <c r="H577">
+        <v>1</v>
+      </c>
+      <c r="I577">
+        <v>0</v>
+      </c>
+      <c r="J577">
+        <v>0</v>
+      </c>
+      <c r="K577">
+        <v>0</v>
+      </c>
+      <c r="L577">
+        <v>0</v>
+      </c>
+      <c r="M577">
+        <v>17</v>
+      </c>
+      <c r="N577">
+        <v>1</v>
+      </c>
+      <c r="O577">
+        <v>0</v>
+      </c>
+      <c r="P577">
+        <v>21</v>
+      </c>
+      <c r="Q577">
+        <v>0</v>
+      </c>
+      <c r="R577">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="578" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>0</v>
+      </c>
+      <c r="B578" t="s">
+        <v>22</v>
+      </c>
+      <c r="C578" t="s">
+        <v>19</v>
+      </c>
+      <c r="D578" t="s">
+        <v>20</v>
+      </c>
+      <c r="E578">
+        <v>102486</v>
+      </c>
+      <c r="F578">
+        <v>3</v>
+      </c>
+      <c r="G578">
+        <v>0</v>
+      </c>
+      <c r="H578">
+        <v>1</v>
+      </c>
+      <c r="I578">
+        <v>0</v>
+      </c>
+      <c r="J578">
+        <v>0</v>
+      </c>
+      <c r="K578">
+        <v>0</v>
+      </c>
+      <c r="L578">
+        <v>0</v>
+      </c>
+      <c r="M578">
+        <v>19</v>
+      </c>
+      <c r="N578">
+        <v>2</v>
+      </c>
+      <c r="O578">
+        <v>0</v>
+      </c>
+      <c r="P578">
+        <v>25</v>
+      </c>
+      <c r="Q578">
+        <v>0</v>
+      </c>
+      <c r="R578">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="579" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>0</v>
+      </c>
+      <c r="B579" t="s">
+        <v>22</v>
+      </c>
+      <c r="C579" t="s">
+        <v>19</v>
+      </c>
+      <c r="D579" t="s">
+        <v>20</v>
+      </c>
+      <c r="E579">
+        <v>102486</v>
+      </c>
+      <c r="F579">
+        <v>2</v>
+      </c>
+      <c r="G579">
+        <v>0</v>
+      </c>
+      <c r="H579">
+        <v>1</v>
+      </c>
+      <c r="I579">
+        <v>0</v>
+      </c>
+      <c r="J579">
+        <v>0</v>
+      </c>
+      <c r="K579">
+        <v>0</v>
+      </c>
+      <c r="L579">
+        <v>0</v>
+      </c>
+      <c r="M579">
+        <v>19</v>
+      </c>
+      <c r="N579">
+        <v>3</v>
+      </c>
+      <c r="O579">
+        <v>0</v>
+      </c>
+      <c r="P579">
+        <v>25</v>
+      </c>
+      <c r="Q579">
+        <v>0</v>
+      </c>
+      <c r="R579">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="580" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>0</v>
+      </c>
+      <c r="B580" t="s">
+        <v>22</v>
+      </c>
+      <c r="C580" t="s">
+        <v>19</v>
+      </c>
+      <c r="D580" t="s">
+        <v>20</v>
+      </c>
+      <c r="E580">
+        <v>102486</v>
+      </c>
+      <c r="F580">
+        <v>4</v>
+      </c>
+      <c r="G580">
+        <v>0</v>
+      </c>
+      <c r="H580">
+        <v>1</v>
+      </c>
+      <c r="I580">
+        <v>1</v>
+      </c>
+      <c r="J580">
+        <v>0</v>
+      </c>
+      <c r="K580">
+        <v>0</v>
+      </c>
+      <c r="L580">
+        <v>0</v>
+      </c>
+      <c r="M580">
+        <v>19</v>
+      </c>
+      <c r="N580">
+        <v>4</v>
+      </c>
+      <c r="O580">
+        <v>0</v>
+      </c>
+      <c r="P580">
+        <v>29</v>
+      </c>
+      <c r="Q580">
+        <v>0</v>
+      </c>
+      <c r="R580">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="581" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>0</v>
+      </c>
+      <c r="B581" t="s">
+        <v>22</v>
+      </c>
+      <c r="C581" t="s">
+        <v>19</v>
+      </c>
+      <c r="D581" t="s">
+        <v>20</v>
+      </c>
+      <c r="E581">
+        <v>102486</v>
+      </c>
+      <c r="F581">
+        <v>3</v>
+      </c>
+      <c r="G581">
+        <v>0</v>
+      </c>
+      <c r="H581">
+        <v>1</v>
+      </c>
+      <c r="I581">
+        <v>1</v>
+      </c>
+      <c r="J581">
+        <v>0</v>
+      </c>
+      <c r="K581">
+        <v>0</v>
+      </c>
+      <c r="L581">
+        <v>0</v>
+      </c>
+      <c r="M581">
+        <v>17</v>
+      </c>
+      <c r="N581">
+        <v>2</v>
+      </c>
+      <c r="O581">
+        <v>0</v>
+      </c>
+      <c r="P581">
+        <v>24</v>
+      </c>
+      <c r="Q581">
+        <v>0</v>
+      </c>
+      <c r="R581">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="582" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>0</v>
+      </c>
+      <c r="B582" t="s">
+        <v>22</v>
+      </c>
+      <c r="C582" t="s">
+        <v>19</v>
+      </c>
+      <c r="D582" t="s">
+        <v>20</v>
+      </c>
+      <c r="E582">
+        <v>102486</v>
+      </c>
+      <c r="F582">
+        <v>2</v>
+      </c>
+      <c r="G582">
+        <v>0</v>
+      </c>
+      <c r="H582">
+        <v>1</v>
+      </c>
+      <c r="I582">
+        <v>1</v>
+      </c>
+      <c r="J582">
+        <v>0</v>
+      </c>
+      <c r="K582">
+        <v>0</v>
+      </c>
+      <c r="L582">
+        <v>0</v>
+      </c>
+      <c r="M582">
+        <v>22</v>
+      </c>
+      <c r="N582">
+        <v>2</v>
+      </c>
+      <c r="O582">
+        <v>0</v>
+      </c>
+      <c r="P582">
+        <v>28</v>
+      </c>
+      <c r="Q582">
+        <v>0</v>
+      </c>
+      <c r="R582">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="583" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D583" t="s">
+        <v>21</v>
+      </c>
+      <c r="E583">
+        <v>102486</v>
+      </c>
+      <c r="F583">
+        <v>2</v>
+      </c>
+      <c r="G583">
+        <v>0</v>
+      </c>
+      <c r="H583">
+        <v>2</v>
+      </c>
+      <c r="I583">
+        <v>0</v>
+      </c>
+      <c r="J583">
+        <v>0</v>
+      </c>
+      <c r="K583">
+        <v>0</v>
+      </c>
+      <c r="L583">
+        <v>0</v>
+      </c>
+      <c r="M583">
+        <v>13</v>
+      </c>
+      <c r="N583">
+        <v>3</v>
+      </c>
+      <c r="O583">
+        <v>0</v>
+      </c>
+      <c r="P583">
+        <v>20</v>
+      </c>
+      <c r="Q583">
+        <v>0</v>
+      </c>
+      <c r="R583">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>